<commit_message>
Update BOM_PartType-Integrated Stepper Motor Driver.xlsx
</commit_message>
<xml_diff>
--- a/HyperRail/PCB Files/Integrated Stepper Motor Driver/BOM/BOM_PartType-Integrated Stepper Motor Driver.xlsx
+++ b/HyperRail/PCB Files/Integrated Stepper Motor Driver/BOM/BOM_PartType-Integrated Stepper Motor Driver.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9FCFD82-9709-46F8-9D88-28F24634CB2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Bruslind\Documents\GitHub\PersonalProjects\HyperRail\PCB Files\Integrated Stepper Motor Driver\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160A4211-2EDC-44CA-AB71-6424AF210DC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="19170" windowHeight="10170" xr2:uid="{3F7F2804-6865-49DA-9CB9-E467399E9372}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3F7F2804-6865-49DA-9CB9-E467399E9372}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Integrated Stepper" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="104">
   <si>
     <t>Capacitance</t>
   </si>
@@ -329,13 +334,25 @@
   </si>
   <si>
     <t>CMP-3786467-11</t>
+  </si>
+  <si>
+    <t>54601-906WPLF</t>
+  </si>
+  <si>
+    <t>1825057-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMC2209-LA-T </t>
+  </si>
+  <si>
+    <t>LMZM23601V5SILR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +363,12 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -391,13 +414,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,7 +741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30646D7C-2EF8-4895-A69B-9F8D754CCE64}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -939,8 +968,8 @@
       <c r="F7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
+      <c r="G7" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -971,8 +1000,8 @@
       <c r="F8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
+      <c r="G8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
@@ -1099,8 +1128,8 @@
       <c r="F12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>17</v>
+      <c r="G12" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
@@ -1163,8 +1192,8 @@
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>17</v>
+      <c r="G14" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1195,8 +1224,8 @@
       <c r="F15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>17</v>
+      <c r="G15" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
update PCBs to be better
</commit_message>
<xml_diff>
--- a/HyperRail/PCB Files/Integrated Stepper Motor Driver/BOM/BOM_PartType-Integrated Stepper Motor Driver.xlsx
+++ b/HyperRail/PCB Files/Integrated Stepper Motor Driver/BOM/BOM_PartType-Integrated Stepper Motor Driver.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E883A8D-091F-434A-B112-7AEA0756F7F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\PCB Files\Integrated Stepper Motor Driver\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A85873-CD4A-4E40-9517-A37DD780E793}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="4860" windowWidth="19170" windowHeight="10170" xr2:uid="{BCB82684-6DCD-4C45-A122-EB82C73E6F19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E41B48D0-9B2B-447C-B94C-255A6E81B237}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Integrated Stepper" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
   <si>
     <t>Capacitance</t>
   </si>
@@ -380,13 +385,34 @@
   </si>
   <si>
     <t>CMP-3786467-11</t>
+  </si>
+  <si>
+    <t>54601-906WPLF</t>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70</t>
+  </si>
+  <si>
+    <t>CRGCQ0603J470R</t>
+  </si>
+  <si>
+    <t>1-1825059-2</t>
+  </si>
+  <si>
+    <t>TMC2209-LA-T</t>
+  </si>
+  <si>
+    <t>LMZM23601V5SILR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‎SBR80520LT1G‎ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,8 +426,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +445,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -439,18 +477,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -762,10 +804,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EB9EAF-4A76-4B93-BEEB-3E281191F774}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599356C5-86D0-41C2-A06C-63457F6D67DA}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -830,7 +874,7 @@
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="3">
@@ -862,7 +906,7 @@
       <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="3">
@@ -894,7 +938,7 @@
       <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="3">
@@ -926,7 +970,7 @@
       <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H5" s="3">
@@ -958,7 +1002,7 @@
       <c r="F6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>44</v>
       </c>
       <c r="H6" s="3">
@@ -990,7 +1034,7 @@
       <c r="F7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H7" s="3">
@@ -1022,15 +1066,12 @@
       <c r="F8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
+      <c r="G8" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1054,8 +1095,8 @@
       <c r="F9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
+      <c r="G9" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -1086,7 +1127,7 @@
       <c r="F10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="H10" s="3">
@@ -1118,7 +1159,7 @@
       <c r="F11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="5" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="3">
@@ -1150,7 +1191,7 @@
       <c r="F12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>74</v>
       </c>
       <c r="H12" s="3">
@@ -1182,8 +1223,8 @@
       <c r="F13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>10</v>
+      <c r="G13" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -1214,8 +1255,8 @@
       <c r="F14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>10</v>
+      <c r="G14" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1246,8 +1287,8 @@
       <c r="F15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>10</v>
+      <c r="G15" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
@@ -1278,7 +1319,7 @@
       <c r="F16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="5" t="s">
         <v>101</v>
       </c>
       <c r="H16" s="3">
@@ -1310,8 +1351,8 @@
       <c r="F17" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
+      <c r="G17" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
@@ -1342,8 +1383,8 @@
       <c r="F18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>10</v>
+      <c r="G18" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
@@ -1374,8 +1415,8 @@
       <c r="F19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>112</v>
+      <c r="G19" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="H19" s="3">
         <v>2</v>

</xml_diff>